<commit_message>
Modificando algunas cositas uu
</commit_message>
<xml_diff>
--- a/RepMasVendidos.xlsx
+++ b/RepMasVendidos.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Reporte de Mas Vendidos</t>
   </si>
@@ -32,31 +32,40 @@
     <t>Stand de los Besos 1</t>
   </si>
   <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Las Aventuras de Paolo y Badboy</t>
+  </si>
+  <si>
     <t>8</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Las Aventuras de Paolo y Badboy</t>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Thor Ragnarod</t>
   </si>
   <si>
     <t>4</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Thor Ragnarod</t>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Stand de los Besos 3</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>La Casa de Papel Temporada 1</t>
   </si>
   <si>
     <t>Stand de los Besos 2</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>Stand de los Besos 3</t>
   </si>
 </sst>
 </file>
@@ -182,7 +191,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:D10"/>
+  <dimension ref="A2:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true" zoomScale="150"/>
   </sheetViews>
@@ -238,29 +247,40 @@
         <v>11</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>